<commit_message>
Lagt till artikelnummer och inköpsantal
</commit_message>
<xml_diff>
--- a/Electronics/MF/BOMv1.xlsx
+++ b/Electronics/MF/BOMv1.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vigurt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\TSTE93_Slutsteget\Electronics\MF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D6BE1432-C0A5-4828-8BF9-ABB51220C338}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD60C9D0-C842-4945-83C6-F551130A1361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slutstegbomhejhopp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="169">
   <si>
     <t>Qty</t>
   </si>
@@ -464,13 +475,76 @@
   </si>
   <si>
     <t>power supply</t>
+  </si>
+  <si>
+    <t>143-54-312</t>
+  </si>
+  <si>
+    <t>160-59-753</t>
+  </si>
+  <si>
+    <t>301-51-488</t>
+  </si>
+  <si>
+    <t>160-59-729</t>
+  </si>
+  <si>
+    <t>300-86-421</t>
+  </si>
+  <si>
+    <t>300-31-719</t>
+  </si>
+  <si>
+    <t>801-5353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELFA/RS Art-nr </t>
+  </si>
+  <si>
+    <t>301-67-967</t>
+  </si>
+  <si>
+    <t>160-59-705</t>
+  </si>
+  <si>
+    <t>300-86-416</t>
+  </si>
+  <si>
+    <t>788-3054</t>
+  </si>
+  <si>
+    <t>160-59-736</t>
+  </si>
+  <si>
+    <t>301-81-579</t>
+  </si>
+  <si>
+    <t>300-86-471</t>
+  </si>
+  <si>
+    <t>913-1009</t>
+  </si>
+  <si>
+    <t>300-18-763</t>
+  </si>
+  <si>
+    <t>173-46-232</t>
+  </si>
+  <si>
+    <t>301-22-457</t>
+  </si>
+  <si>
+    <t>165-57-664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOQ +20% </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,6 +702,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF979797"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -972,11 +1060,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1332,27 +1422,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="148.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="148.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1381,13 +1471,19 @@
         <v>134</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1416,15 +1512,18 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <f>I2*G2</f>
         <v>9.7899999999999991</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1453,15 +1552,18 @@
       <c r="I3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>I3*G3</f>
         <v>11.27</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
@@ -1490,15 +1592,18 @@
       <c r="I4">
         <v>25</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J35" si="1">I4*G4</f>
+      <c r="K4">
+        <f t="shared" ref="K4:K35" si="1">I4*G4</f>
         <v>16.48</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>19</v>
       </c>
@@ -1527,15 +1632,18 @@
       <c r="I5">
         <v>100</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>11.27</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1564,15 +1672,18 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>14.680000000000001</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -1601,15 +1712,18 @@
       <c r="I7">
         <v>12</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>23.52</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1638,15 +1752,18 @@
       <c r="I8">
         <v>25</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="1"/>
         <v>32.975000000000001</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1675,15 +1792,15 @@
       <c r="I9">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>5.82</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1712,15 +1829,18 @@
       <c r="I10">
         <v>10</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>10.4</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1749,15 +1869,18 @@
       <c r="I11">
         <v>2</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f t="shared" si="1"/>
         <v>0.22120000000000001</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1786,15 +1909,18 @@
       <c r="I12">
         <v>100</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="1"/>
         <v>14.11</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1823,15 +1949,18 @@
       <c r="I13">
         <v>11</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="1"/>
         <v>23.572999999999997</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1860,15 +1989,18 @@
       <c r="I14">
         <v>100</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="1"/>
         <v>11.27</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1897,15 +2029,18 @@
       <c r="I15">
         <v>50</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="1"/>
         <v>13.020000000000001</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1934,15 +2069,18 @@
       <c r="I16">
         <v>100</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>9.98</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1971,15 +2109,15 @@
       <c r="I17">
         <v>4</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="1"/>
         <v>17.28</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2008,15 +2146,15 @@
       <c r="I18">
         <v>4</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f t="shared" si="1"/>
         <v>74.8</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2045,15 +2183,15 @@
       <c r="I19">
         <v>2</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>16.12</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2082,15 +2220,15 @@
       <c r="I20">
         <v>4</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f t="shared" si="1"/>
         <v>31.24</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2113,13 +2251,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2145,15 +2283,18 @@
       <c r="I22">
         <v>5</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f t="shared" si="1"/>
         <v>50.11</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2182,15 +2323,18 @@
       <c r="I23">
         <v>5</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f t="shared" si="1"/>
         <v>30.75</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2219,15 +2363,18 @@
       <c r="I24">
         <v>10</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f t="shared" si="1"/>
         <v>37.599999999999994</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2253,15 +2400,15 @@
       <c r="I25">
         <v>3</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f t="shared" si="1"/>
         <v>31.17</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2287,15 +2434,15 @@
       <c r="I26">
         <v>3</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f t="shared" si="1"/>
         <v>30.42</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2324,15 +2471,18 @@
       <c r="I27">
         <v>4</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f t="shared" si="1"/>
         <v>55.2</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="L27" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2361,15 +2511,15 @@
       <c r="I28">
         <v>1</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f t="shared" si="1"/>
         <v>3.49</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2398,15 +2548,15 @@
       <c r="I29">
         <v>1</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <f t="shared" si="1"/>
         <v>2.99</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2429,12 +2579,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2463,15 +2613,15 @@
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f t="shared" si="1"/>
         <v>46.95</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2500,26 +2650,26 @@
       <c r="I32">
         <v>1</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <f t="shared" si="1"/>
         <v>63.9</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H33">
         <f t="shared" ref="H33:H35" si="2">G33*A33</f>
         <v>0</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2539,15 +2689,18 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <f t="shared" si="1"/>
         <v>20.7</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="L34" t="s">
+        <v>166</v>
+      </c>
+      <c r="M34" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2567,15 +2720,15 @@
       <c r="I35">
         <v>1</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f t="shared" si="1"/>
         <v>332.4</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="M35" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>SUM(A2:A32)</f>
         <v>152</v>
@@ -2587,62 +2740,63 @@
       <c r="I36" t="s">
         <v>137</v>
       </c>
-      <c r="J36">
-        <f>SUM(J2:J35)</f>
+      <c r="K36">
+        <f>SUM(K2:K35)</f>
         <v>1053.4992000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I37" t="s">
         <v>138</v>
       </c>
-      <c r="J37">
-        <f>SUM(J3,J4,J5,J6,J7,J8,J10,J11,J12,J13,J14,J15,J16,J22,J23,J24,J27,J2,J34)</f>
+      <c r="K37">
+        <f>SUM(K3,K4,K5,K6,K7,K8,K10,K11,K12,K13,K14,K15,K16,K22,K23,K24,K27,K2,K34)</f>
         <v>396.91919999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I38" t="s">
         <v>139</v>
       </c>
-      <c r="J38">
-        <f>J36-J37</f>
+      <c r="K38">
+        <f>K36-K37</f>
         <v>656.58000000000015</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="K4" r:id="rId2"/>
-    <hyperlink ref="K5" r:id="rId3"/>
-    <hyperlink ref="K8" r:id="rId4"/>
-    <hyperlink ref="K9" r:id="rId5"/>
-    <hyperlink ref="K18" r:id="rId6"/>
-    <hyperlink ref="K17" r:id="rId7"/>
-    <hyperlink ref="K6" r:id="rId8"/>
-    <hyperlink ref="K7" r:id="rId9"/>
-    <hyperlink ref="K10" r:id="rId10"/>
-    <hyperlink ref="K11" r:id="rId11"/>
-    <hyperlink ref="K12" r:id="rId12"/>
-    <hyperlink ref="K13" r:id="rId13"/>
-    <hyperlink ref="K14" r:id="rId14"/>
-    <hyperlink ref="K15" r:id="rId15"/>
-    <hyperlink ref="K16" r:id="rId16"/>
-    <hyperlink ref="K19" r:id="rId17"/>
-    <hyperlink ref="K20" r:id="rId18"/>
-    <hyperlink ref="K22" r:id="rId19"/>
-    <hyperlink ref="K23" r:id="rId20"/>
-    <hyperlink ref="K24" r:id="rId21"/>
-    <hyperlink ref="K25" r:id="rId22"/>
-    <hyperlink ref="K26" r:id="rId23"/>
-    <hyperlink ref="K27" r:id="rId24"/>
-    <hyperlink ref="K28" r:id="rId25"/>
-    <hyperlink ref="K29" r:id="rId26"/>
-    <hyperlink ref="K31" r:id="rId27"/>
-    <hyperlink ref="K32" r:id="rId28"/>
-    <hyperlink ref="K34" r:id="rId29"/>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="M17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="M7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="M13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="M14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="M15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="M19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="M20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="M22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="M24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="M26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="M28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="M31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="M34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="M2" r:id="rId30" xr:uid="{2DAE2CB2-54FF-49C2-AEBB-A22DAD8FA2DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uppdaterad och skickad till Arta
Skickad de poster som var till ELFA och RS.  Uppdaterad nya kolumner för inköp med marginal. Måste göra klart de vi köper själva från Digikey
</commit_message>
<xml_diff>
--- a/Electronics/MF/BOMv1.xlsx
+++ b/Electronics/MF/BOMv1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\TSTE93_Slutsteget\Electronics\MF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD60C9D0-C842-4945-83C6-F551130A1361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7CA7EE-A17C-4929-BBF7-30140459DE84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7044" yWindow="648" windowWidth="23040" windowHeight="13728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slutstegbomhejhopp" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="177">
   <si>
     <t>Qty</t>
   </si>
@@ -537,7 +537,31 @@
     <t>165-57-664</t>
   </si>
   <si>
-    <t xml:space="preserve">MOQ +20% </t>
+    <t xml:space="preserve">MOQ + marginal </t>
+  </si>
+  <si>
+    <t>SW0</t>
+  </si>
+  <si>
+    <t>PDB182-K430K-503A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/products/en?keywords=PDB182-K430K-503A</t>
+  </si>
+  <si>
+    <t>DUAL POT 50K OHM 0.06W CARBON LOG</t>
+  </si>
+  <si>
+    <t>MOQ-ext-Marginal</t>
+  </si>
+  <si>
+    <t>3.5mm 3pole audio connector</t>
+  </si>
+  <si>
+    <t>POT 50K OHM 0.06W CARBON LOG</t>
+  </si>
+  <si>
+    <t>FERRIT</t>
   </si>
 </sst>
 </file>
@@ -718,7 +742,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,6 +920,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1060,13 +1096,16 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1423,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1438,11 +1477,15 @@
     <col min="6" max="6" width="44.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="18.44140625" customWidth="1"/>
-    <col min="13" max="13" width="148.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="12" max="12" width="23.5546875" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="148.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1477,13 +1520,16 @@
         <v>136</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1506,24 +1552,31 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="H2">
-        <f>G2*A2</f>
+        <f t="shared" ref="H2:H36" si="0">G2*A2</f>
         <v>9.7899999999999991</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
       <c r="K2">
-        <f>I2*G2</f>
+        <f t="shared" ref="K2:K36" si="1">I2*G2</f>
         <v>9.7899999999999991</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2">
+        <f t="shared" ref="L2:L36" si="2">J2*G2</f>
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1546,24 +1599,31 @@
         <v>0.11269999999999999</v>
       </c>
       <c r="H3">
-        <f>G3*A3</f>
+        <f t="shared" si="0"/>
         <v>0.67619999999999991</v>
       </c>
       <c r="I3">
         <v>100</v>
       </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
       <c r="K3">
-        <f>I3*G3</f>
+        <f t="shared" si="1"/>
         <v>11.27</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3">
+        <f t="shared" si="2"/>
+        <v>11.27</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
@@ -1586,24 +1646,31 @@
         <v>0.65920000000000001</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H31" si="0">G4*A4</f>
+        <f t="shared" si="0"/>
         <v>10.5472</v>
       </c>
       <c r="I4">
         <v>25</v>
       </c>
+      <c r="J4">
+        <v>25</v>
+      </c>
       <c r="K4">
-        <f t="shared" ref="K4:K35" si="1">I4*G4</f>
+        <f t="shared" si="1"/>
         <v>16.48</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>16.48</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>19</v>
       </c>
@@ -1632,18 +1699,25 @@
       <c r="I5">
         <v>100</v>
       </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
       <c r="K5">
         <f t="shared" si="1"/>
         <v>11.27</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>11.27</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1672,18 +1746,25 @@
       <c r="I6">
         <v>100</v>
       </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
       <c r="K6">
         <f t="shared" si="1"/>
         <v>14.680000000000001</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>14.680000000000001</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -1712,18 +1793,25 @@
       <c r="I7">
         <v>12</v>
       </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
       <c r="K7">
         <f t="shared" si="1"/>
         <v>23.52</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>29.4</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1752,55 +1840,69 @@
       <c r="I8">
         <v>25</v>
       </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
       <c r="K8">
         <f t="shared" si="1"/>
         <v>32.975000000000001</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>32.975000000000001</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>2.91</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <f t="shared" si="0"/>
         <v>5.82</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="6">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="J9" s="6">
+        <v>4</v>
+      </c>
+      <c r="K9" s="6">
         <f t="shared" si="1"/>
         <v>5.82</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="L9" s="6">
+        <f t="shared" si="2"/>
+        <v>11.64</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1829,18 +1931,25 @@
       <c r="I10">
         <v>10</v>
       </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
       <c r="K10">
         <f t="shared" si="1"/>
         <v>10.4</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>10.4</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1869,18 +1978,25 @@
       <c r="I11">
         <v>2</v>
       </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
       <c r="K11">
         <f t="shared" si="1"/>
         <v>0.22120000000000001</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1909,18 +2025,25 @@
       <c r="I12">
         <v>100</v>
       </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
       <c r="K12">
         <f t="shared" si="1"/>
         <v>14.11</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>14.11</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1949,18 +2072,25 @@
       <c r="I13">
         <v>11</v>
       </c>
+      <c r="J13">
+        <v>14</v>
+      </c>
       <c r="K13">
         <f t="shared" si="1"/>
         <v>23.572999999999997</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>30.001999999999995</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1989,18 +2119,25 @@
       <c r="I14">
         <v>100</v>
       </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
       <c r="K14">
         <f t="shared" si="1"/>
         <v>11.27</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>11.27</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2029,18 +2166,25 @@
       <c r="I15">
         <v>50</v>
       </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
       <c r="K15">
         <f t="shared" si="1"/>
         <v>13.020000000000001</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>13.020000000000001</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2069,195 +2213,237 @@
       <c r="I16">
         <v>100</v>
       </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
       <c r="K16">
         <f t="shared" si="1"/>
         <v>9.98</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>9.98</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <v>4.32</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="6">
         <f t="shared" si="0"/>
         <v>17.28</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="6">
         <v>4</v>
       </c>
-      <c r="K17">
+      <c r="J17" s="6">
+        <v>5</v>
+      </c>
+      <c r="K17" s="6">
         <f t="shared" si="1"/>
         <v>17.28</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="L17" s="6">
+        <f t="shared" si="2"/>
+        <v>21.6</v>
+      </c>
+      <c r="N17" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>74477010</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>74477010</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <v>18.7</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="6">
         <f t="shared" si="0"/>
         <v>74.8</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="6">
         <v>4</v>
       </c>
-      <c r="K18">
+      <c r="J18" s="6">
+        <v>5</v>
+      </c>
+      <c r="K18" s="6">
         <f t="shared" si="1"/>
         <v>74.8</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="L18" s="6">
+        <f t="shared" si="2"/>
+        <v>93.5</v>
+      </c>
+      <c r="N18" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="19" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="6">
         <v>8.06</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="6">
         <f t="shared" si="0"/>
         <v>16.12</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="6">
         <v>2</v>
       </c>
-      <c r="K19">
+      <c r="J19" s="6">
+        <v>4</v>
+      </c>
+      <c r="K19" s="6">
         <f t="shared" si="1"/>
         <v>16.12</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="L19" s="6">
+        <f t="shared" si="2"/>
+        <v>32.24</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="6">
         <v>7.81</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="6">
         <f t="shared" si="0"/>
         <v>31.24</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="6">
         <v>4</v>
       </c>
-      <c r="K20">
+      <c r="J20" s="6">
+        <v>5</v>
+      </c>
+      <c r="K20" s="6">
         <f t="shared" si="1"/>
         <v>31.24</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="L20" s="6">
+        <f t="shared" si="2"/>
+        <v>39.049999999999997</v>
+      </c>
+      <c r="N20" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
+      <c r="J21" s="6">
         <v>0</v>
       </c>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K21" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2273,6 +2459,9 @@
       <c r="E22" t="s">
         <v>55</v>
       </c>
+      <c r="F22" s="6" t="s">
+        <v>174</v>
+      </c>
       <c r="G22">
         <v>10.022</v>
       </c>
@@ -2283,18 +2472,25 @@
       <c r="I22">
         <v>5</v>
       </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
       <c r="K22">
         <f t="shared" si="1"/>
         <v>50.11</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>50.11</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2323,18 +2519,25 @@
       <c r="I23">
         <v>5</v>
       </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
       <c r="K23">
         <f t="shared" si="1"/>
         <v>30.75</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>30.75</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="N23" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2363,86 +2566,110 @@
       <c r="I24">
         <v>10</v>
       </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
       <c r="K24">
         <f t="shared" si="1"/>
         <v>37.599999999999994</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>37.599999999999994</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
         <v>3</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="6">
         <v>10.39</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="6">
         <f t="shared" si="0"/>
         <v>31.17</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="6">
         <v>3</v>
       </c>
-      <c r="K25">
+      <c r="J25" s="6">
+        <v>3</v>
+      </c>
+      <c r="K25" s="6">
         <f t="shared" si="1"/>
         <v>31.17</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="L25" s="6">
+        <f t="shared" si="2"/>
+        <v>31.17</v>
+      </c>
+      <c r="N25" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G26">
+      <c r="F26" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="6">
         <v>10.14</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>30.42</v>
-      </c>
-      <c r="I26">
-        <v>3</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="1"/>
-        <v>30.42</v>
-      </c>
-      <c r="M26" s="2" t="s">
+      <c r="H26" s="6">
+        <f t="shared" si="0"/>
+        <v>10.14</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="1"/>
+        <v>10.14</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="2"/>
+        <v>10.14</v>
+      </c>
+      <c r="N26" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2471,205 +2698,251 @@
       <c r="I27">
         <v>4</v>
       </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
       <c r="K27">
         <f t="shared" si="1"/>
         <v>55.2</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="M27" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>1</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="6">
         <v>3.49</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="6">
         <f t="shared" si="0"/>
         <v>3.49</v>
       </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="K28">
+      <c r="I28" s="6">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6">
+        <v>1</v>
+      </c>
+      <c r="K28" s="6">
         <f t="shared" si="1"/>
         <v>3.49</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="L28" s="6">
+        <f t="shared" si="2"/>
+        <v>3.49</v>
+      </c>
+      <c r="N28" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>1</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <v>2.99</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="6">
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="K29">
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+      <c r="K29" s="6">
         <f t="shared" si="1"/>
         <v>2.99</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="L29" s="6">
+        <f t="shared" si="2"/>
+        <v>2.99</v>
+      </c>
+      <c r="N29" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="30" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="1"/>
+      <c r="J30" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="K30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="6">
         <v>46.95</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="6">
         <f t="shared" si="0"/>
         <v>46.95</v>
       </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="K31">
+      <c r="I31" s="6">
+        <v>1</v>
+      </c>
+      <c r="J31" s="6">
+        <v>1</v>
+      </c>
+      <c r="K31" s="6">
         <f t="shared" si="1"/>
         <v>46.95</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="L31" s="6">
+        <f t="shared" si="2"/>
+        <v>46.95</v>
+      </c>
+      <c r="N31" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="32" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>1</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="6">
         <v>63.9</v>
       </c>
-      <c r="H32">
-        <f>G32*A32</f>
+      <c r="H32" s="6">
+        <f t="shared" si="0"/>
         <v>63.9</v>
       </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="K32">
+      <c r="I32" s="6">
+        <v>1</v>
+      </c>
+      <c r="J32" s="6">
+        <v>1</v>
+      </c>
+      <c r="K32" s="6">
         <f t="shared" si="1"/>
         <v>63.9</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="L32" s="6">
+        <f t="shared" si="2"/>
+        <v>63.9</v>
+      </c>
+      <c r="N32" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H33">
-        <f t="shared" ref="H33:H35" si="2">G33*A33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2683,120 +2956,191 @@
         <v>20.7</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20.7</v>
       </c>
       <c r="I34">
         <v>1</v>
       </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
       <c r="K34">
         <f t="shared" si="1"/>
         <v>20.7</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>20.7</v>
+      </c>
+      <c r="M34" t="s">
         <v>166</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="35" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="6">
         <v>332.4</v>
       </c>
-      <c r="H35">
-        <f t="shared" si="2"/>
+      <c r="H35" s="6">
+        <f t="shared" si="0"/>
         <v>332.4</v>
       </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="K35">
+      <c r="I35" s="6">
+        <v>1</v>
+      </c>
+      <c r="J35" s="6">
+        <v>1</v>
+      </c>
+      <c r="K35" s="6">
         <f t="shared" si="1"/>
         <v>332.4</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="L35" s="6">
+        <f t="shared" si="2"/>
+        <v>332.4</v>
+      </c>
+      <c r="N35" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="36" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="6">
+        <v>15.87</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" si="0"/>
+        <v>15.87</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1</v>
+      </c>
+      <c r="J36" s="6">
+        <v>1</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" si="1"/>
+        <v>15.87</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="2"/>
+        <v>15.87</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F37" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38">
         <f>SUM(A2:A32)</f>
-        <v>152</v>
-      </c>
-      <c r="H36">
+        <v>150</v>
+      </c>
+      <c r="H38">
         <f>SUM(H2:H32)</f>
-        <v>487.74590000000001</v>
-      </c>
-      <c r="I36" t="s">
+        <v>467.46589999999998</v>
+      </c>
+      <c r="I38" t="s">
         <v>137</v>
       </c>
-      <c r="K36">
-        <f>SUM(K2:K35)</f>
-        <v>1053.4992000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I37" t="s">
+      <c r="K38">
+        <f>SUM(K2:K36)</f>
+        <v>1049.0891999999999</v>
+      </c>
+      <c r="L38">
+        <f>SUM(L2:L36)</f>
+        <v>1128.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
         <v>138</v>
       </c>
-      <c r="K37">
+      <c r="K39">
         <f>SUM(K3,K4,K5,K6,K7,K8,K10,K11,K12,K13,K14,K15,K16,K22,K23,K24,K27,K2,K34)</f>
         <v>396.91919999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I38" t="s">
+      <c r="L39">
+        <f>SUM(L3,L4,L5,L6,L7,L8,L10,L11,L12,L13,L14,L15,L16,L22,L23,L24,L27,L2,L34)</f>
+        <v>423.36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
         <v>139</v>
       </c>
-      <c r="K38">
-        <f>K36-K37</f>
-        <v>656.58000000000015</v>
+      <c r="K40">
+        <f>K38-K39</f>
+        <v>652.16999999999985</v>
+      </c>
+      <c r="L40">
+        <f>L38-L39</f>
+        <v>704.93999999999994</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="M4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="M5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="M8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="M9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="M18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="M17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="M6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="M7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="M10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="M11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="M12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="M13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="M14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="M15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="M16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="M19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="M20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="M22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="M23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="M24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="M25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="M26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="M27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="M28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="M29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="M31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="M32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="M34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="M2" r:id="rId30" xr:uid="{2DAE2CB2-54FF-49C2-AEBB-A22DAD8FA2DD}"/>
+    <hyperlink ref="N3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="N18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="N17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="N7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="N10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="N11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="N13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="N14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="N15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="N16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="N19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="N20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="N22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="N23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="N24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="N25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="N26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="N27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="N28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="N29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="N31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="N32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="N34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="N2" r:id="rId30" xr:uid="{2DAE2CB2-54FF-49C2-AEBB-A22DAD8FA2DD}"/>
+    <hyperlink ref="N36" r:id="rId31" xr:uid="{4FB16334-6B9C-4D81-9FA6-96631708493A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lagt till mer rader i BOMEN
</commit_message>
<xml_diff>
--- a/Electronics/MF/BOMv1.xlsx
+++ b/Electronics/MF/BOMv1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\TSTE93_Slutsteget\Electronics\MF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7CA7EE-A17C-4929-BBF7-30140459DE84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071B094E-EDF3-4033-8ACB-3AD1AA65FFE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7044" yWindow="648" windowWidth="23040" windowHeight="13728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slutstegbomhejhopp" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="195">
   <si>
     <t>Qty</t>
   </si>
@@ -540,9 +540,6 @@
     <t xml:space="preserve">MOQ + marginal </t>
   </si>
   <si>
-    <t>SW0</t>
-  </si>
-  <si>
     <t>PDB182-K430K-503A</t>
   </si>
   <si>
@@ -562,6 +559,63 @@
   </si>
   <si>
     <t>FERRIT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/product-detail/en/jst-sales-america-inc/VHR-4M/455-3990-ND/9924201?cur=SEK&amp;lang=en</t>
+  </si>
+  <si>
+    <t>PVDD connector Hona</t>
+  </si>
+  <si>
+    <t>VHR-4M</t>
+  </si>
+  <si>
+    <t>B4P-VH(LF)(SN)</t>
+  </si>
+  <si>
+    <t>PVDD connector Hane</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/product-detail/en/jst-sales-america-inc/B4P-VH-LF-SN/455-1641-ND/926549?cur=SEK&amp;lang=en</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/products/en?keywords=ASVHSVH16K152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Black 16 AWG Jumper Lead Socket to Socket Tin 6.00" </t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/products/en?keywords=TG-A6200-10-5-0.5</t>
+  </si>
+  <si>
+    <t>TG-A6200-10-5-0.5</t>
+  </si>
+  <si>
+    <t>Thermal Pad</t>
+  </si>
+  <si>
+    <t>HA40101V4-1000U-A99</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/products/en?keywords=HA40101V4-1000U-A99</t>
+  </si>
+  <si>
+    <t>Fan Tubeaxial 12VDC Square - 40mm L x 40mm</t>
+  </si>
+  <si>
+    <t>V5618C</t>
+  </si>
+  <si>
+    <t>HEATSINK ALUM ANOD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/products/en?keywords=V5618C</t>
+  </si>
+  <si>
+    <t>Crimpade PVDD kablar</t>
+  </si>
+  <si>
+    <t>SW?</t>
   </si>
 </sst>
 </file>
@@ -742,7 +796,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -931,6 +985,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,7 +1156,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
@@ -1106,6 +1166,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1462,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,7 +1581,7 @@
         <v>136</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>155</v>
@@ -1552,7 +1613,7 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H36" si="0">G2*A2</f>
+        <f t="shared" ref="H2:H37" si="0">G2*A2</f>
         <v>9.7899999999999991</v>
       </c>
       <c r="I2">
@@ -2460,7 +2521,7 @@
         <v>55</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G22">
         <v>10.022</v>
@@ -2642,7 +2703,7 @@
         <v>69</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G26" s="6">
         <v>10.14</v>
@@ -3020,13 +3081,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>170</v>
-      </c>
       <c r="F36" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G36" s="6">
         <v>15.87</v>
@@ -3050,59 +3111,155 @@
         <v>15.87</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
       <c r="F37" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>178</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G39" s="6">
+        <v>2.41</v>
+      </c>
+      <c r="N39" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="N37" s="2"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>183</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G40" s="6">
+        <v>5.65</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>185</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>187</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G42" s="6">
+        <v>22.6</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>190</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="6">
+        <v>7.15</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
         <f>SUM(A2:A32)</f>
         <v>150</v>
       </c>
-      <c r="H38">
+      <c r="H44">
         <f>SUM(H2:H32)</f>
         <v>467.46589999999998</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I44" t="s">
         <v>137</v>
       </c>
-      <c r="K38">
+      <c r="K44">
         <f>SUM(K2:K36)</f>
         <v>1049.0891999999999</v>
       </c>
-      <c r="L38">
+      <c r="L44">
         <f>SUM(L2:L36)</f>
         <v>1128.3</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I39" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
         <v>138</v>
       </c>
-      <c r="K39">
+      <c r="K45">
         <f>SUM(K3,K4,K5,K6,K7,K8,K10,K11,K12,K13,K14,K15,K16,K22,K23,K24,K27,K2,K34)</f>
         <v>396.91919999999999</v>
       </c>
-      <c r="L39">
+      <c r="L45">
         <f>SUM(L3,L4,L5,L6,L7,L8,L10,L11,L12,L13,L14,L15,L16,L22,L23,L24,L27,L2,L34)</f>
         <v>423.36</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I40" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
         <v>139</v>
       </c>
-      <c r="K40">
-        <f>K38-K39</f>
+      <c r="K46">
+        <f>K44-K45</f>
         <v>652.16999999999985</v>
       </c>
-      <c r="L40">
-        <f>L38-L39</f>
+      <c r="L46">
+        <f>L44-L45</f>
         <v>704.93999999999994</v>
       </c>
     </row>
@@ -3139,8 +3296,12 @@
     <hyperlink ref="N34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="N2" r:id="rId30" xr:uid="{2DAE2CB2-54FF-49C2-AEBB-A22DAD8FA2DD}"/>
     <hyperlink ref="N36" r:id="rId31" xr:uid="{4FB16334-6B9C-4D81-9FA6-96631708493A}"/>
+    <hyperlink ref="N39" r:id="rId32" xr:uid="{22DAF23A-9B74-4D2E-803B-63E91B07E7E5}"/>
+    <hyperlink ref="N41" r:id="rId33" xr:uid="{504204DC-C26C-4EE2-82E7-A52607E5E8D0}"/>
+    <hyperlink ref="N42" r:id="rId34" xr:uid="{56A7C5C0-FB97-407E-ADE9-5957BEF88B02}"/>
+    <hyperlink ref="N43" r:id="rId35" xr:uid="{605FCDEE-731C-44D7-AEFA-5C2E7B7A4524}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uppdaterat lite extra poster
</commit_message>
<xml_diff>
--- a/Electronics/MF/BOMv1.xlsx
+++ b/Electronics/MF/BOMv1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\TSTE93_Slutsteget\Electronics\MF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071B094E-EDF3-4033-8ACB-3AD1AA65FFE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F83D961-7E52-4839-AB03-0DE7A423A80F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="197">
   <si>
     <t>Qty</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>SW?</t>
+  </si>
+  <si>
+    <t>APT15DQ60KG</t>
+  </si>
+  <si>
+    <t>https://www.digikey.se/products/sv?keywords=APT15DQ60KG</t>
   </si>
 </sst>
 </file>
@@ -1523,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3115,7 +3121,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
+      <c r="A37" s="9"/>
       <c r="F37" s="8" t="s">
         <v>175</v>
       </c>
@@ -3127,7 +3133,8 @@
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D38" t="s">
+      <c r="A38" s="9"/>
+      <c r="C38" t="s">
         <v>179</v>
       </c>
       <c r="F38" s="9" t="s">
@@ -3147,7 +3154,8 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D39" t="s">
+      <c r="A39" s="9"/>
+      <c r="C39" t="s">
         <v>178</v>
       </c>
       <c r="F39" s="9" t="s">
@@ -3161,7 +3169,8 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D40" t="s">
+      <c r="A40" s="9"/>
+      <c r="C40" t="s">
         <v>183</v>
       </c>
       <c r="F40" s="9" t="s">
@@ -3175,7 +3184,8 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D41" t="s">
+      <c r="A41" s="9"/>
+      <c r="C41" t="s">
         <v>185</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -3189,7 +3199,8 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D42" t="s">
+      <c r="A42" s="9"/>
+      <c r="C42" t="s">
         <v>187</v>
       </c>
       <c r="F42" s="9" t="s">
@@ -3203,7 +3214,8 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D43" t="s">
+      <c r="A43" s="9"/>
+      <c r="C43" t="s">
         <v>190</v>
       </c>
       <c r="F43" s="9" t="s">
@@ -3217,49 +3229,64 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="9"/>
+      <c r="C44" t="s">
+        <v>195</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G44" s="6">
+        <v>4.49</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45">
         <f>SUM(A2:A32)</f>
         <v>150</v>
       </c>
-      <c r="H44">
+      <c r="H45">
         <f>SUM(H2:H32)</f>
         <v>467.46589999999998</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>137</v>
       </c>
-      <c r="K44">
+      <c r="K45">
         <f>SUM(K2:K36)</f>
         <v>1049.0891999999999</v>
       </c>
-      <c r="L44">
+      <c r="L45">
         <f>SUM(L2:L36)</f>
         <v>1128.3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I45" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
         <v>138</v>
       </c>
-      <c r="K45">
+      <c r="K46">
         <f>SUM(K3,K4,K5,K6,K7,K8,K10,K11,K12,K13,K14,K15,K16,K22,K23,K24,K27,K2,K34)</f>
         <v>396.91919999999999</v>
       </c>
-      <c r="L45">
+      <c r="L46">
         <f>SUM(L3,L4,L5,L6,L7,L8,L10,L11,L12,L13,L14,L15,L16,L22,L23,L24,L27,L2,L34)</f>
         <v>423.36</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I46" t="s">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
         <v>139</v>
       </c>
-      <c r="K46">
-        <f>K44-K45</f>
+      <c r="K47">
+        <f>K45-K46</f>
         <v>652.16999999999985</v>
       </c>
-      <c r="L46">
-        <f>L44-L45</f>
+      <c r="L47">
+        <f>L45-L46</f>
         <v>704.93999999999994</v>
       </c>
     </row>
@@ -3300,8 +3327,9 @@
     <hyperlink ref="N41" r:id="rId33" xr:uid="{504204DC-C26C-4EE2-82E7-A52607E5E8D0}"/>
     <hyperlink ref="N42" r:id="rId34" xr:uid="{56A7C5C0-FB97-407E-ADE9-5957BEF88B02}"/>
     <hyperlink ref="N43" r:id="rId35" xr:uid="{605FCDEE-731C-44D7-AEFA-5C2E7B7A4524}"/>
+    <hyperlink ref="N44" r:id="rId36" xr:uid="{462E7D61-EA78-421F-B931-3A76FF60B194}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixade stavfel i BOM
</commit_message>
<xml_diff>
--- a/Electronics/MF/BOMv1.xlsx
+++ b/Electronics/MF/BOMv1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\TSTE93_Slutsteget\Electronics\MF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F83D961-7E52-4839-AB03-0DE7A423A80F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82C1F50-4812-498F-A45E-208D63EFF166}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="198">
   <si>
     <t>Qty</t>
   </si>
@@ -622,6 +622,9 @@
   </si>
   <si>
     <t>https://www.digikey.se/products/sv?keywords=APT15DQ60KG</t>
+  </si>
+  <si>
+    <t>Värm-upp-huset-Dioder</t>
   </si>
 </sst>
 </file>
@@ -1531,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3234,7 +3237,7 @@
         <v>195</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G44" s="6">
         <v>4.49</v>

</xml_diff>

<commit_message>
Pillar lite med ny BOM
Fortfarande lite rörigt
</commit_message>
<xml_diff>
--- a/Electronics/MF/BOMv1.xlsx
+++ b/Electronics/MF/BOMv1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\GitHub\TSTE93_Slutsteget\Electronics\MF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC1DFDE-A277-4B1F-8DC4-B24BFF79429B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EA8F79-4529-49F6-92AF-07E1977D521A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24072" yWindow="4752" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slutstegbomhejhopp" sheetId="1" r:id="rId1"/>
@@ -1534,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,7 +1622,7 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H37" si="0">G2*A2</f>
+        <f>G2*A2</f>
         <v>9.7899999999999991</v>
       </c>
       <c r="I2">
@@ -1632,11 +1632,11 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K36" si="1">I2*G2</f>
+        <f>I2*G2</f>
         <v>9.7899999999999991</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:L36" si="2">J2*G2</f>
+        <f>J2*G2</f>
         <v>9.7899999999999991</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -1669,7 +1669,7 @@
         <v>0.11269999999999999</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f>G3*A3</f>
         <v>0.67619999999999991</v>
       </c>
       <c r="I3">
@@ -1679,11 +1679,11 @@
         <v>100</v>
       </c>
       <c r="K3">
-        <f t="shared" si="1"/>
+        <f>I3*G3</f>
         <v>11.27</v>
       </c>
       <c r="L3">
-        <f t="shared" si="2"/>
+        <f>J3*G3</f>
         <v>11.27</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -1716,7 +1716,7 @@
         <v>0.65920000000000001</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>G4*A4</f>
         <v>10.5472</v>
       </c>
       <c r="I4">
@@ -1726,11 +1726,11 @@
         <v>25</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f>I4*G4</f>
         <v>16.48</v>
       </c>
       <c r="L4">
-        <f t="shared" si="2"/>
+        <f>J4*G4</f>
         <v>16.48</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -1763,7 +1763,7 @@
         <v>0.11269999999999999</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f>G5*A5</f>
         <v>2.1412999999999998</v>
       </c>
       <c r="I5">
@@ -1773,11 +1773,11 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f>I5*G5</f>
         <v>11.27</v>
       </c>
       <c r="L5">
-        <f t="shared" si="2"/>
+        <f>J5*G5</f>
         <v>11.27</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -1810,7 +1810,7 @@
         <v>0.14680000000000001</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>G6*A6</f>
         <v>1.1744000000000001</v>
       </c>
       <c r="I6">
@@ -1820,11 +1820,11 @@
         <v>100</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f>I6*G6</f>
         <v>14.680000000000001</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f>J6*G6</f>
         <v>14.680000000000001</v>
       </c>
       <c r="M6" s="4" t="s">
@@ -1857,7 +1857,7 @@
         <v>1.96</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>G7*A7</f>
         <v>23.52</v>
       </c>
       <c r="I7">
@@ -1867,11 +1867,11 @@
         <v>15</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f>I7*G7</f>
         <v>23.52</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f>J7*G7</f>
         <v>29.4</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -1904,7 +1904,7 @@
         <v>1.319</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>G8*A8</f>
         <v>1.319</v>
       </c>
       <c r="I8">
@@ -1914,11 +1914,11 @@
         <v>25</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f>I8*G8</f>
         <v>32.975000000000001</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f>J8*G8</f>
         <v>32.975000000000001</v>
       </c>
       <c r="M8" s="5" t="s">
@@ -1951,7 +1951,7 @@
         <v>2.91</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="0"/>
+        <f>G9*A9</f>
         <v>5.82</v>
       </c>
       <c r="I9" s="6">
@@ -1961,11 +1961,11 @@
         <v>4</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="1"/>
+        <f>I9*G9</f>
         <v>5.82</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="2"/>
+        <f>J9*G9</f>
         <v>11.64</v>
       </c>
       <c r="N9" s="7" t="s">
@@ -1995,7 +1995,7 @@
         <v>1.04</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f>G10*A10</f>
         <v>2.08</v>
       </c>
       <c r="I10">
@@ -2005,11 +2005,11 @@
         <v>10</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f>I10*G10</f>
         <v>10.4</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f>J10*G10</f>
         <v>10.4</v>
       </c>
       <c r="M10" s="4" t="s">
@@ -2042,7 +2042,7 @@
         <v>0.1106</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f>G11*A11</f>
         <v>0.22120000000000001</v>
       </c>
       <c r="I11">
@@ -2052,11 +2052,11 @@
         <v>5</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f>I11*G11</f>
         <v>0.22120000000000001</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f>J11*G11</f>
         <v>0.55300000000000005</v>
       </c>
       <c r="M11" s="4" t="s">
@@ -2089,7 +2089,7 @@
         <v>0.1411</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f>G12*A12</f>
         <v>1.6932</v>
       </c>
       <c r="I12">
@@ -2099,11 +2099,11 @@
         <v>100</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f>I12*G12</f>
         <v>14.11</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f>J12*G12</f>
         <v>14.11</v>
       </c>
       <c r="M12" s="4" t="s">
@@ -2136,7 +2136,7 @@
         <v>2.1429999999999998</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f>G13*A13</f>
         <v>23.572999999999997</v>
       </c>
       <c r="I13">
@@ -2146,11 +2146,11 @@
         <v>14</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f>I13*G13</f>
         <v>23.572999999999997</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f>J13*G13</f>
         <v>30.001999999999995</v>
       </c>
       <c r="M13" s="5" t="s">
@@ -2183,7 +2183,7 @@
         <v>0.11269999999999999</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f>G14*A14</f>
         <v>0.67619999999999991</v>
       </c>
       <c r="I14">
@@ -2193,11 +2193,11 @@
         <v>100</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f>I14*G14</f>
         <v>11.27</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f>J14*G14</f>
         <v>11.27</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -2230,7 +2230,7 @@
         <v>0.26040000000000002</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f>G15*A15</f>
         <v>2.6040000000000001</v>
       </c>
       <c r="I15">
@@ -2240,11 +2240,11 @@
         <v>50</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f>I15*G15</f>
         <v>13.020000000000001</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f>J15*G15</f>
         <v>13.020000000000001</v>
       </c>
       <c r="M15" s="4" t="s">
@@ -2277,7 +2277,7 @@
         <v>9.98E-2</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f>G16*A16</f>
         <v>0.8982</v>
       </c>
       <c r="I16">
@@ -2287,11 +2287,11 @@
         <v>100</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f>I16*G16</f>
         <v>9.98</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f>J16*G16</f>
         <v>9.98</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -2324,7 +2324,7 @@
         <v>4.32</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="0"/>
+        <f>G17*A17</f>
         <v>17.28</v>
       </c>
       <c r="I17" s="6">
@@ -2334,11 +2334,11 @@
         <v>5</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="1"/>
+        <f>I17*G17</f>
         <v>17.28</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="2"/>
+        <f>J17*G17</f>
         <v>21.6</v>
       </c>
       <c r="N17" s="7" t="s">
@@ -2368,7 +2368,7 @@
         <v>18.7</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="0"/>
+        <f>G18*A18</f>
         <v>74.8</v>
       </c>
       <c r="I18" s="6">
@@ -2378,11 +2378,11 @@
         <v>5</v>
       </c>
       <c r="K18" s="6">
-        <f t="shared" si="1"/>
+        <f>I18*G18</f>
         <v>74.8</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="2"/>
+        <f>J18*G18</f>
         <v>93.5</v>
       </c>
       <c r="N18" s="7" t="s">
@@ -2412,7 +2412,7 @@
         <v>8.06</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="0"/>
+        <f>G19*A19</f>
         <v>16.12</v>
       </c>
       <c r="I19" s="6">
@@ -2422,11 +2422,11 @@
         <v>4</v>
       </c>
       <c r="K19" s="6">
-        <f t="shared" si="1"/>
+        <f>I19*G19</f>
         <v>16.12</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="2"/>
+        <f>J19*G19</f>
         <v>32.24</v>
       </c>
       <c r="N19" s="7" t="s">
@@ -2456,7 +2456,7 @@
         <v>7.81</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="0"/>
+        <f>G20*A20</f>
         <v>31.24</v>
       </c>
       <c r="I20" s="6">
@@ -2466,11 +2466,11 @@
         <v>5</v>
       </c>
       <c r="K20" s="6">
-        <f t="shared" si="1"/>
+        <f>I20*G20</f>
         <v>31.24</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="2"/>
+        <f>J20*G20</f>
         <v>39.049999999999997</v>
       </c>
       <c r="N20" s="7" t="s">
@@ -2497,18 +2497,18 @@
         <v>54</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="0"/>
+        <f>G21*A21</f>
         <v>0</v>
       </c>
       <c r="J21" s="6">
         <v>0</v>
       </c>
       <c r="K21" s="6">
-        <f t="shared" si="1"/>
+        <f>I21*G21</f>
         <v>0</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="2"/>
+        <f>J21*G21</f>
         <v>0</v>
       </c>
       <c r="N21" s="7"/>
@@ -2536,7 +2536,7 @@
         <v>10.022</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f>G22*A22</f>
         <v>10.022</v>
       </c>
       <c r="I22">
@@ -2546,11 +2546,11 @@
         <v>5</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f>I22*G22</f>
         <v>50.11</v>
       </c>
       <c r="L22">
-        <f t="shared" si="2"/>
+        <f>J22*G22</f>
         <v>50.11</v>
       </c>
       <c r="M22" s="5" t="s">
@@ -2583,7 +2583,7 @@
         <v>6.15</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f>G23*A23</f>
         <v>6.15</v>
       </c>
       <c r="I23">
@@ -2593,11 +2593,11 @@
         <v>5</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
+        <f>I23*G23</f>
         <v>30.75</v>
       </c>
       <c r="L23">
-        <f t="shared" si="2"/>
+        <f>J23*G23</f>
         <v>30.75</v>
       </c>
       <c r="M23" s="4" t="s">
@@ -2630,7 +2630,7 @@
         <v>3.76</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f>G24*A24</f>
         <v>11.28</v>
       </c>
       <c r="I24">
@@ -2640,11 +2640,11 @@
         <v>10</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
+        <f>I24*G24</f>
         <v>37.599999999999994</v>
       </c>
       <c r="L24">
-        <f t="shared" si="2"/>
+        <f>J24*G24</f>
         <v>37.599999999999994</v>
       </c>
       <c r="M24" s="4" t="s">
@@ -2674,7 +2674,7 @@
         <v>10.39</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="0"/>
+        <f>G25*A25</f>
         <v>31.17</v>
       </c>
       <c r="I25" s="6">
@@ -2684,11 +2684,11 @@
         <v>3</v>
       </c>
       <c r="K25" s="6">
-        <f t="shared" si="1"/>
+        <f>I25*G25</f>
         <v>31.17</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="2"/>
+        <f>J25*G25</f>
         <v>31.17</v>
       </c>
       <c r="N25" s="7" t="s">
@@ -2718,7 +2718,7 @@
         <v>10.14</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="0"/>
+        <f>G26*A26</f>
         <v>10.14</v>
       </c>
       <c r="I26" s="6">
@@ -2728,11 +2728,11 @@
         <v>1</v>
       </c>
       <c r="K26" s="6">
-        <f t="shared" si="1"/>
+        <f>I26*G26</f>
         <v>10.14</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="2"/>
+        <f>J26*G26</f>
         <v>10.14</v>
       </c>
       <c r="N26" s="7" t="s">
@@ -2762,7 +2762,7 @@
         <v>13.8</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f>G27*A27</f>
         <v>55.2</v>
       </c>
       <c r="I27">
@@ -2772,11 +2772,11 @@
         <v>5</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f>I27*G27</f>
         <v>55.2</v>
       </c>
       <c r="L27">
-        <f t="shared" si="2"/>
+        <f>J27*G27</f>
         <v>69</v>
       </c>
       <c r="M27" s="4" t="s">
@@ -2809,7 +2809,7 @@
         <v>3.49</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="0"/>
+        <f>G28*A28</f>
         <v>3.49</v>
       </c>
       <c r="I28" s="6">
@@ -2819,11 +2819,11 @@
         <v>1</v>
       </c>
       <c r="K28" s="6">
-        <f t="shared" si="1"/>
+        <f>I28*G28</f>
         <v>3.49</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="2"/>
+        <f>J28*G28</f>
         <v>3.49</v>
       </c>
       <c r="N28" s="7" t="s">
@@ -2853,7 +2853,7 @@
         <v>2.99</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="0"/>
+        <f>G29*A29</f>
         <v>2.99</v>
       </c>
       <c r="I29" s="6">
@@ -2863,11 +2863,11 @@
         <v>1</v>
       </c>
       <c r="K29" s="6">
-        <f t="shared" si="1"/>
+        <f>I29*G29</f>
         <v>2.99</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="2"/>
+        <f>J29*G29</f>
         <v>2.99</v>
       </c>
       <c r="N29" s="7" t="s">
@@ -2894,18 +2894,18 @@
         <v>85</v>
       </c>
       <c r="H30" s="6">
-        <f t="shared" si="0"/>
+        <f>G30*A30</f>
         <v>0</v>
       </c>
       <c r="J30" s="6">
         <v>0</v>
       </c>
       <c r="K30" s="6">
-        <f t="shared" si="1"/>
+        <f>I30*G30</f>
         <v>0</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="2"/>
+        <f>J30*G30</f>
         <v>0</v>
       </c>
     </row>
@@ -2932,7 +2932,7 @@
         <v>46.95</v>
       </c>
       <c r="H31" s="6">
-        <f t="shared" si="0"/>
+        <f>G31*A31</f>
         <v>46.95</v>
       </c>
       <c r="I31" s="6">
@@ -2942,11 +2942,11 @@
         <v>1</v>
       </c>
       <c r="K31" s="6">
-        <f t="shared" si="1"/>
+        <f>I31*G31</f>
         <v>46.95</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="2"/>
+        <f>J31*G31</f>
         <v>46.95</v>
       </c>
       <c r="N31" s="7" t="s">
@@ -2976,7 +2976,7 @@
         <v>63.9</v>
       </c>
       <c r="H32" s="6">
-        <f t="shared" si="0"/>
+        <f>G32*A32</f>
         <v>63.9</v>
       </c>
       <c r="I32" s="6">
@@ -2986,11 +2986,11 @@
         <v>1</v>
       </c>
       <c r="K32" s="6">
-        <f t="shared" si="1"/>
+        <f>I32*G32</f>
         <v>63.9</v>
       </c>
       <c r="L32" s="6">
-        <f t="shared" si="2"/>
+        <f>J32*G32</f>
         <v>63.9</v>
       </c>
       <c r="N32" s="7" t="s">
@@ -2999,15 +2999,15 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f>G33*A33</f>
         <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f>I33*G33</f>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="shared" si="2"/>
+        <f>J33*G33</f>
         <v>0</v>
       </c>
       <c r="N33" s="2"/>
@@ -3026,7 +3026,7 @@
         <v>20.7</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
+        <f>G34*A34</f>
         <v>20.7</v>
       </c>
       <c r="I34">
@@ -3036,11 +3036,11 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f>I34*G34</f>
         <v>20.7</v>
       </c>
       <c r="L34">
-        <f t="shared" si="2"/>
+        <f>J34*G34</f>
         <v>20.7</v>
       </c>
       <c r="M34" t="s">
@@ -3064,7 +3064,7 @@
         <v>332.4</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" si="0"/>
+        <f>G35*A35</f>
         <v>332.4</v>
       </c>
       <c r="I35" s="6">
@@ -3074,11 +3074,11 @@
         <v>1</v>
       </c>
       <c r="K35" s="6">
-        <f t="shared" si="1"/>
+        <f>I35*G35</f>
         <v>332.4</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="2"/>
+        <f>J35*G35</f>
         <v>332.4</v>
       </c>
       <c r="N35" s="7" t="s">
@@ -3102,7 +3102,7 @@
         <v>15.87</v>
       </c>
       <c r="H36" s="6">
-        <f t="shared" si="0"/>
+        <f>G36*A36</f>
         <v>15.87</v>
       </c>
       <c r="I36" s="6">
@@ -3112,11 +3112,11 @@
         <v>1</v>
       </c>
       <c r="K36" s="6">
-        <f t="shared" si="1"/>
+        <f>I36*G36</f>
         <v>15.87</v>
       </c>
       <c r="L36" s="6">
-        <f t="shared" si="2"/>
+        <f>J36*G36</f>
         <v>15.87</v>
       </c>
       <c r="N36" s="7" t="s">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6">
-        <f t="shared" si="0"/>
+        <f>G37*A37</f>
         <v>0</v>
       </c>
       <c r="N37" s="2"/>
@@ -3331,8 +3331,9 @@
     <hyperlink ref="N42" r:id="rId34" xr:uid="{56A7C5C0-FB97-407E-ADE9-5957BEF88B02}"/>
     <hyperlink ref="N43" r:id="rId35" xr:uid="{605FCDEE-731C-44D7-AEFA-5C2E7B7A4524}"/>
     <hyperlink ref="N44" r:id="rId36" xr:uid="{462E7D61-EA78-421F-B931-3A76FF60B194}"/>
+    <hyperlink ref="N38" r:id="rId37" xr:uid="{509AC6B3-37A9-49ED-A3F5-E1EFB2C2888A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>